<commit_message>
Pull Transltions for local project de, es
</commit_message>
<xml_diff>
--- a/i18n/de/translations.xlsx
+++ b/i18n/de/translations.xlsx
@@ -30,29 +30,392 @@
 </metadata>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
+  <si>
+    <t>Table 2681651900 - Field 883711285 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Eintrags-Nr.</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 3948098573 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Anzahl der Erinnerungen</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 3710982960 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Buchungsdatum</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 580412389 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Belegdatum</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 4085727052 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Fälligkeitsdatum</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 2363328873 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Belegart</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 486908828 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Beleg-Nr.</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 3461834954 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Beschreibung</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 1077555671 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Ursprünglicher Betrag</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 2975378708 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Restbetrag</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 4200184881 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Nr.</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 636392376 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Betrag</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 1213267064 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Zinssatz</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 2139693550 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Allgemeine Produktbuchungsgruppe</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 1246077090 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>USt %</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 2971014054 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>USt-Berechnungstyp</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 1108276017 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>USt-Betrag</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 2552458873 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Steuergruppencode</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 236064653 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>USt-Produktbuchungsgruppe</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 2534656220 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>USt-Identifikator</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 158172202 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Zeilentyp</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 158172202 - Property 62802879</t>
+  </si>
+  <si>
+    <t>Erinnerungszeile,Fälligkeitsdatum,Anfangstext,Endtext,Rundung,Ausgesetzt,Zusatzgebühr,Zeilenggebühr</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 2162283589 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>USt-Klauselcode</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 400684573 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Belegart, auf die angewandt wird</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 677070472 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Beleg-Nr., auf die angewandt wird</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 1746606869 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Eintrag mit detaillierten Zinssätzen</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - Field 2283884360 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Systemerstellter Eintrag</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - NamedType 4094643921</t>
+  </si>
+  <si>
+    <t>Der %1 auf dem %2 und der %3 müssen gleich sein.</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - NamedType 1984498423</t>
+  </si>
+  <si>
+    <t>%1 muss %2 oder %3 sein.</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - NamedType 3593856238</t>
+  </si>
+  <si>
+    <t>Es gibt kein offenes %1 mit %2 %3.</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - NamedType 3459220650</t>
+  </si>
+  <si>
+    <t>%1 %2 in %3 ist nicht überfällig.</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - NamedType 659963034</t>
+  </si>
+  <si>
+    <t>Die Zeilenentgelt für %1 %2 auf Erinnerungsebene %3 wurde bereits ausgestelt.</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - NamedType 885110970</t>
+  </si>
+  <si>
+    <t>%1 muss positiv sein.</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - NamedType 2618258002</t>
+  </si>
+  <si>
+    <t>Es gibt nicht genug Platz, um Zeilen mit zusätzlichen Zinssätzen einzufügen.</t>
+  </si>
+  <si>
+    <t>Table 2681651900 - NamedType 2800588376</t>
+  </si>
+  <si>
+    <t>Erstellen Sie einen Zinssatz mit einem Startdatum vor %1.</t>
+  </si>
+  <si>
+    <t>Table 3280694829 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Erinnerungsbedingungen</t>
+  </si>
+  <si>
+    <t>Table 3280694829 - Field 3004954119 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Table 3280694829 - Field 3461834954 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Table 3280694829 - Field 2757499274 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Zinsen buchen</t>
+  </si>
+  <si>
+    <t>Table 3280694829 - Field 3274756825 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Zusätzliche Gebühr buchen</t>
+  </si>
+  <si>
+    <t>Table 3280694829 - Field 55421187 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Maximale Anzahl an Erinnerungen</t>
+  </si>
+  <si>
+    <t>Table 3280694829 - Field 650382431 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Mindestbetrag (LCY)</t>
+  </si>
+  <si>
+    <t>Table 3280694829 - Field 3410685676 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Zusatzgebühr pro Zeile buchen</t>
+  </si>
+  <si>
+    <t>Table 3280694829 - Field 2009106446 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Hinweis zur Zeilenggebühr im Bericht</t>
+  </si>
+  <si>
+    <t>Page 3280694829 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Page 3280694829 - Control 3004954119 - Property 1295455071</t>
+  </si>
+  <si>
+    <t>Gibt einen Code an, um dieses Set von Erinnerungskonditionen zu identifizieren.</t>
+  </si>
+  <si>
+    <t>Page 3280694829 - Control 3461834954 - Property 1295455071</t>
+  </si>
+  <si>
+    <t>Gibt eine Beschreibung der Erinnerungskonditionen an.</t>
+  </si>
+  <si>
+    <t>Page 3280694829 - Control 55421187 - Property 1295455071</t>
+  </si>
+  <si>
+    <t>Gibt die maximale Anzahl an Erinnerungen an, die für eine Rechnung erstellt werden können.</t>
+  </si>
+  <si>
+    <t>Page 3280694829 - Control 2757499274 - Property 1295455071</t>
+  </si>
+  <si>
+    <t>Gibt an, ob die auf der Erinnerung aufgeführte Zinsen im Hauptbuch und den Kundenkonten gebucht werden sollen oder nicht.</t>
+  </si>
+  <si>
+    <t>Page 3280694829 - Control 3274756825 - Property 1295455071</t>
+  </si>
+  <si>
+    <t>Gibt an, ob die auf der Erinnerung aufgeführte zusätzliche Gebühr im Hauptbuch und den Kundenkonten gebucht werden soll oder nicht.</t>
+  </si>
+  <si>
+    <t>Page 3280694829 - Control 3410685676 - Property 1295455071</t>
+  </si>
+  <si>
+    <t>Gibt an, ob die auf der Finanzierungskostenmitteilung aufgeführte zusätzliche Gebühr im Hauptbuch und den Kundenkonten gebucht werden soll, wenn die Mitteilung ausgestellt wird.</t>
+  </si>
+  <si>
+    <t>Page 3280694829 - Control 650382431 - Property 1295455071</t>
+  </si>
+  <si>
+    <t>Gibt den Mindestbetrag an, für den eine Erinnerung erstellt wird.</t>
+  </si>
+  <si>
+    <t>Page 3280694829 - Control 2009106446 - Property 1295455071</t>
+  </si>
+  <si>
+    <t>Gibt an, dass alle Hinweise zu Zeilenkosten der Erinnerung hinzugefügt werden.</t>
+  </si>
+  <si>
+    <t>Page 3280694829 - Action 2050659749 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>&amp;Ebenen</t>
+  </si>
+  <si>
+    <t>Page 3280694829 - Action 2050659749 - Property 1295455071</t>
+  </si>
+  <si>
+    <t>Zeigen Sie die Erinnerungsebenen an, die verwendet werden, um zu definieren, wann Erinnerungen erstellt werden können und welche Gebühren und Texte sie enthalten müssen.</t>
+  </si>
+  <si>
+    <t>Page 3280694829 - Action 1358710565 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Übersetzung</t>
+  </si>
+  <si>
+    <t>Page 3280694829 - Action 1358710565 - Property 1295455071</t>
+  </si>
+  <si>
+    <t>Zeigen Sie den Erinnerungstext in allen anderen Sprachen an, die für Erinnerungen eingerichtet sind.</t>
+  </si>
+  <si>
+    <t>Table 1909723412 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Übersetzung der Erinnerungskonditionen</t>
+  </si>
+  <si>
+    <t>Table 1909723412 - Field 1840439778 - Property 2879900210</t>
+  </si>
+  <si>
+    <t>Erinnerungsbedingungen-Code</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
+      <sz val="11"/>
       <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill patternType="none">
+        <bgColor/>
+      </patternFill>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="gray125">
+        <bgColor/>
+      </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -61,13 +424,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="1" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="true"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -397,38 +765,486 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B59"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
-      <c r="A1" t="str">
-        <v>Key</v>
-      </c>
-      <c r="B1" t="str">
-        <v>Translation</v>
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="str">
-        <v>welcome</v>
-      </c>
-      <c r="B2" t="str">
-        <v>Bienvenido</v>
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="str">
-        <v>goodbye</v>
-      </c>
-      <c r="B3" t="str">
-        <v>Adiós</v>
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B59"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
yes we creating prs now
</commit_message>
<xml_diff>
--- a/i18n/de/translations.xlsx
+++ b/i18n/de/translations.xlsx
@@ -31,7 +31,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="120">
+  <si>
+    <t>only one</t>
+  </si>
+  <si>
+    <t>dafrett</t>
+  </si>
+  <si>
+    <t>another empty</t>
+  </si>
+  <si>
+    <t>Beispieltext</t>
+  </si>
   <si>
     <t>Table 2681651900 - Field 883711285 - Property 2879900210</t>
   </si>
@@ -114,25 +126,25 @@
     <t>Table 2681651900 - Field 2139693550 - Property 2879900210</t>
   </si>
   <si>
-    <t>Allgemeine Produktbuchungsgruppe</t>
+    <t>Allg. Produkterfassungsgruppe</t>
   </si>
   <si>
     <t>Table 2681651900 - Field 1246077090 - Property 2879900210</t>
   </si>
   <si>
-    <t>USt %</t>
+    <t>Mehrwertsteuer %</t>
   </si>
   <si>
     <t>Table 2681651900 - Field 2971014054 - Property 2879900210</t>
   </si>
   <si>
-    <t>USt-Berechnungstyp</t>
+    <t>Mehrwertsteuer-Berechnungsart</t>
   </si>
   <si>
     <t>Table 2681651900 - Field 1108276017 - Property 2879900210</t>
   </si>
   <si>
-    <t>USt-Betrag</t>
+    <t>Mehrwertsteuerbetrag</t>
   </si>
   <si>
     <t>Table 2681651900 - Field 2552458873 - Property 2879900210</t>
@@ -144,61 +156,61 @@
     <t>Table 2681651900 - Field 236064653 - Property 2879900210</t>
   </si>
   <si>
-    <t>USt-Produktbuchungsgruppe</t>
+    <t>Mehrwertsteuer-Produktermittlungsgruppe</t>
   </si>
   <si>
     <t>Table 2681651900 - Field 2534656220 - Property 2879900210</t>
   </si>
   <si>
-    <t>USt-Identifikator</t>
+    <t>Mehrwertsteuer-Identifikator</t>
   </si>
   <si>
     <t>Table 2681651900 - Field 158172202 - Property 2879900210</t>
   </si>
   <si>
-    <t>Zeilentyp</t>
+    <t>Leitungstyp</t>
   </si>
   <si>
     <t>Table 2681651900 - Field 158172202 - Property 62802879</t>
   </si>
   <si>
-    <t>Erinnerungszeile,Fälligkeitsdatum,Anfangstext,Endtext,Rundung,Ausgesetzt,Zusatzgebühr,Zeilenggebühr</t>
+    <t>Erinnerungszeile, Nicht fällig, Anfangstext, Endtext, Rundung, In Wartestellung, Zusatzgebühr, Leitungsgebühr</t>
   </si>
   <si>
     <t>Table 2681651900 - Field 2162283589 - Property 2879900210</t>
   </si>
   <si>
-    <t>USt-Klauselcode</t>
+    <t>Mehrwertsteuerklauselcode</t>
   </si>
   <si>
     <t>Table 2681651900 - Field 400684573 - Property 2879900210</t>
   </si>
   <si>
-    <t>Belegart, auf die angewandt wird</t>
+    <t>Zugehörige Belegart</t>
   </si>
   <si>
     <t>Table 2681651900 - Field 677070472 - Property 2879900210</t>
   </si>
   <si>
-    <t>Beleg-Nr., auf die angewandt wird</t>
+    <t>Zugehörige Beleg-Nr.</t>
   </si>
   <si>
     <t>Table 2681651900 - Field 1746606869 - Property 2879900210</t>
   </si>
   <si>
-    <t>Eintrag mit detaillierten Zinssätzen</t>
+    <t>Eingabe der detaillierten Zinssätze</t>
   </si>
   <si>
     <t>Table 2681651900 - Field 2283884360 - Property 2879900210</t>
   </si>
   <si>
-    <t>Systemerstellter Eintrag</t>
+    <t>Systemerzeugter Eintrag</t>
   </si>
   <si>
     <t>Table 2681651900 - NamedType 4094643921</t>
   </si>
   <si>
-    <t>Der %1 auf dem %2 und der %3 müssen gleich sein.</t>
+    <t>Das %1 auf dem %2 und das %3 müssen gleich sein.</t>
   </si>
   <si>
     <t>Table 2681651900 - NamedType 1984498423</t>
@@ -222,7 +234,7 @@
     <t>Table 2681651900 - NamedType 659963034</t>
   </si>
   <si>
-    <t>Die Zeilenentgelt für %1 %2 auf Erinnerungsebene %3 wurde bereits ausgestelt.</t>
+    <t>Die Leitungsgebühr für %1 %2 auf Erinnerungsebene %3 wurde bereits ausgestellt.</t>
   </si>
   <si>
     <t>Table 2681651900 - NamedType 885110970</t>
@@ -234,7 +246,7 @@
     <t>Table 2681651900 - NamedType 2618258002</t>
   </si>
   <si>
-    <t>Es gibt nicht genug Platz, um Zeilen mit zusätzlichen Zinssätzen einzufügen.</t>
+    <t>Es gibt nicht genügend Platz, um Zeilen mit zusätzlichen Zinssätzen einzufügen.</t>
   </si>
   <si>
     <t>Table 2681651900 - NamedType 2800588376</t>
@@ -267,13 +279,13 @@
     <t>Table 3280694829 - Field 3274756825 - Property 2879900210</t>
   </si>
   <si>
-    <t>Zusätzliche Gebühr buchen</t>
+    <t>Zusatzgebühr buchen</t>
   </si>
   <si>
     <t>Table 3280694829 - Field 55421187 - Property 2879900210</t>
   </si>
   <si>
-    <t>Maximale Anzahl an Erinnerungen</t>
+    <t>Max. Anzahl an Erinnerungen</t>
   </si>
   <si>
     <t>Table 3280694829 - Field 650382431 - Property 2879900210</t>
@@ -291,7 +303,7 @@
     <t>Table 3280694829 - Field 2009106446 - Property 2879900210</t>
   </si>
   <si>
-    <t>Hinweis zur Zeilenggebühr im Bericht</t>
+    <t>Hinweis zur Leitungsgebühr im Bericht</t>
   </si>
   <si>
     <t>Page 3280694829 - Property 2879900210</t>
@@ -318,19 +330,19 @@
     <t>Page 3280694829 - Control 2757499274 - Property 1295455071</t>
   </si>
   <si>
-    <t>Gibt an, ob die auf der Erinnerung aufgeführte Zinsen im Hauptbuch und den Kundenkonten gebucht werden sollen oder nicht.</t>
+    <t>Gibt an, ob die in der Erinnerung aufgeführte Zinsen auf das Hauptbuch und die Kundenkonten gebucht werden sollen oder nicht.</t>
   </si>
   <si>
     <t>Page 3280694829 - Control 3274756825 - Property 1295455071</t>
   </si>
   <si>
-    <t>Gibt an, ob die auf der Erinnerung aufgeführte zusätzliche Gebühr im Hauptbuch und den Kundenkonten gebucht werden soll oder nicht.</t>
+    <t>Gibt an, ob die in der Erinnerung aufgeführte Zusatzgebühr auf das Hauptbuch und die Kundenkonten gebucht werden soll oder nicht.</t>
   </si>
   <si>
     <t>Page 3280694829 - Control 3410685676 - Property 1295455071</t>
   </si>
   <si>
-    <t>Gibt an, ob die auf der Finanzierungskostenmitteilung aufgeführte zusätzliche Gebühr im Hauptbuch und den Kundenkonten gebucht werden soll, wenn die Mitteilung ausgestellt wird.</t>
+    <t>Gibt an, ob die in der Verzugszinsmitteilung aufgeführte Zusatzgebühr auf das Hauptbuch und die Kundenkonten gebucht werden soll oder nicht, wenn die Mitteilung ausgestellt wird.</t>
   </si>
   <si>
     <t>Page 3280694829 - Control 650382431 - Property 1295455071</t>
@@ -342,7 +354,7 @@
     <t>Page 3280694829 - Control 2009106446 - Property 1295455071</t>
   </si>
   <si>
-    <t>Gibt an, dass alle Hinweise zu Zeilenkosten der Erinnerung hinzugefügt werden.</t>
+    <t>Gibt an, dass alle Hinweise zu Gebühren im Zusammenhang mit der Leitungsgebühr in die Erinnerung aufgenommen werden.</t>
   </si>
   <si>
     <t>Page 3280694829 - Action 2050659749 - Property 2879900210</t>
@@ -378,7 +390,7 @@
     <t>Table 1909723412 - Field 1840439778 - Property 2879900210</t>
   </si>
   <si>
-    <t>Erinnerungsbedingungen-Code</t>
+    <t>Erinnerungsbedingungscode</t>
   </si>
 </sst>
 </file>
@@ -765,7 +777,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1071,23 +1083,23 @@
         <v>74</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>78</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41">
@@ -1127,23 +1139,23 @@
         <v>87</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48">
@@ -1242,9 +1254,25 @@
         <v>115</v>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B59"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B61"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
classy till the end
</commit_message>
<xml_diff>
--- a/i18n/de/translations.xlsx
+++ b/i18n/de/translations.xlsx
@@ -31,7 +31,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="120">
+  <si>
+    <t>only one</t>
+  </si>
+  <si>
+    <t>dafrett</t>
+  </si>
+  <si>
+    <t>another empty</t>
+  </si>
+  <si>
+    <t>Beispieltext</t>
+  </si>
   <si>
     <t>Table 2681651900 - Field 883711285 - Property 2879900210</t>
   </si>
@@ -114,25 +126,25 @@
     <t>Table 2681651900 - Field 2139693550 - Property 2879900210</t>
   </si>
   <si>
-    <t>Allgemeine Produktbuchungsgruppe</t>
+    <t>Allg. Produkterfassungsgruppe</t>
   </si>
   <si>
     <t>Table 2681651900 - Field 1246077090 - Property 2879900210</t>
   </si>
   <si>
-    <t>USt %</t>
+    <t>Mehrwertsteuer %</t>
   </si>
   <si>
     <t>Table 2681651900 - Field 2971014054 - Property 2879900210</t>
   </si>
   <si>
-    <t>USt-Berechnungstyp</t>
+    <t>Mehrwertsteuer-Berechnungsart</t>
   </si>
   <si>
     <t>Table 2681651900 - Field 1108276017 - Property 2879900210</t>
   </si>
   <si>
-    <t>USt-Betrag</t>
+    <t>Mehrwertsteuerbetrag</t>
   </si>
   <si>
     <t>Table 2681651900 - Field 2552458873 - Property 2879900210</t>
@@ -144,61 +156,61 @@
     <t>Table 2681651900 - Field 236064653 - Property 2879900210</t>
   </si>
   <si>
-    <t>USt-Produktbuchungsgruppe</t>
+    <t>Mehrwertsteuer-Produktermittlungsgruppe</t>
   </si>
   <si>
     <t>Table 2681651900 - Field 2534656220 - Property 2879900210</t>
   </si>
   <si>
-    <t>USt-Identifikator</t>
+    <t>Mehrwertsteuer-Identifikator</t>
   </si>
   <si>
     <t>Table 2681651900 - Field 158172202 - Property 2879900210</t>
   </si>
   <si>
-    <t>Zeilentyp</t>
+    <t>Leitungstyp</t>
   </si>
   <si>
     <t>Table 2681651900 - Field 158172202 - Property 62802879</t>
   </si>
   <si>
-    <t>Erinnerungszeile,Fälligkeitsdatum,Anfangstext,Endtext,Rundung,Ausgesetzt,Zusatzgebühr,Zeilenggebühr</t>
+    <t>Erinnerungszeile, Nicht fällig, Anfangstext, Endtext, Rundung, In Wartestellung, Zusatzgebühr, Leitungsgebühr</t>
   </si>
   <si>
     <t>Table 2681651900 - Field 2162283589 - Property 2879900210</t>
   </si>
   <si>
-    <t>USt-Klauselcode</t>
+    <t>Mehrwertsteuerklauselcode</t>
   </si>
   <si>
     <t>Table 2681651900 - Field 400684573 - Property 2879900210</t>
   </si>
   <si>
-    <t>Belegart, auf die angewandt wird</t>
+    <t>Zugehörige Belegart</t>
   </si>
   <si>
     <t>Table 2681651900 - Field 677070472 - Property 2879900210</t>
   </si>
   <si>
-    <t>Beleg-Nr., auf die angewandt wird</t>
+    <t>Zugehörige Beleg-Nr.</t>
   </si>
   <si>
     <t>Table 2681651900 - Field 1746606869 - Property 2879900210</t>
   </si>
   <si>
-    <t>Eintrag mit detaillierten Zinssätzen</t>
+    <t>Eingabe der detaillierten Zinssätze</t>
   </si>
   <si>
     <t>Table 2681651900 - Field 2283884360 - Property 2879900210</t>
   </si>
   <si>
-    <t>Systemerstellter Eintrag</t>
+    <t>Systemerzeugter Eintrag</t>
   </si>
   <si>
     <t>Table 2681651900 - NamedType 4094643921</t>
   </si>
   <si>
-    <t>Der %1 auf dem %2 und der %3 müssen gleich sein.</t>
+    <t>Das %1 auf dem %2 und das %3 müssen gleich sein.</t>
   </si>
   <si>
     <t>Table 2681651900 - NamedType 1984498423</t>
@@ -222,7 +234,7 @@
     <t>Table 2681651900 - NamedType 659963034</t>
   </si>
   <si>
-    <t>Die Zeilenentgelt für %1 %2 auf Erinnerungsebene %3 wurde bereits ausgestelt.</t>
+    <t>Die Leitungsgebühr für %1 %2 auf Erinnerungsebene %3 wurde bereits ausgestellt.</t>
   </si>
   <si>
     <t>Table 2681651900 - NamedType 885110970</t>
@@ -234,7 +246,7 @@
     <t>Table 2681651900 - NamedType 2618258002</t>
   </si>
   <si>
-    <t>Es gibt nicht genug Platz, um Zeilen mit zusätzlichen Zinssätzen einzufügen.</t>
+    <t>Es gibt nicht genügend Platz, um Zeilen mit zusätzlichen Zinssätzen einzufügen.</t>
   </si>
   <si>
     <t>Table 2681651900 - NamedType 2800588376</t>
@@ -267,13 +279,13 @@
     <t>Table 3280694829 - Field 3274756825 - Property 2879900210</t>
   </si>
   <si>
-    <t>Zusätzliche Gebühr buchen</t>
+    <t>Zusatzgebühr buchen</t>
   </si>
   <si>
     <t>Table 3280694829 - Field 55421187 - Property 2879900210</t>
   </si>
   <si>
-    <t>Maximale Anzahl an Erinnerungen</t>
+    <t>Max. Anzahl an Erinnerungen</t>
   </si>
   <si>
     <t>Table 3280694829 - Field 650382431 - Property 2879900210</t>
@@ -291,7 +303,7 @@
     <t>Table 3280694829 - Field 2009106446 - Property 2879900210</t>
   </si>
   <si>
-    <t>Hinweis zur Zeilenggebühr im Bericht</t>
+    <t>Hinweis zur Leitungsgebühr im Bericht</t>
   </si>
   <si>
     <t>Page 3280694829 - Property 2879900210</t>
@@ -318,19 +330,19 @@
     <t>Page 3280694829 - Control 2757499274 - Property 1295455071</t>
   </si>
   <si>
-    <t>Gibt an, ob die auf der Erinnerung aufgeführte Zinsen im Hauptbuch und den Kundenkonten gebucht werden sollen oder nicht.</t>
+    <t>Gibt an, ob die in der Erinnerung aufgeführte Zinsen auf das Hauptbuch und die Kundenkonten gebucht werden sollen oder nicht.</t>
   </si>
   <si>
     <t>Page 3280694829 - Control 3274756825 - Property 1295455071</t>
   </si>
   <si>
-    <t>Gibt an, ob die auf der Erinnerung aufgeführte zusätzliche Gebühr im Hauptbuch und den Kundenkonten gebucht werden soll oder nicht.</t>
+    <t>Gibt an, ob die in der Erinnerung aufgeführte Zusatzgebühr auf das Hauptbuch und die Kundenkonten gebucht werden soll oder nicht.</t>
   </si>
   <si>
     <t>Page 3280694829 - Control 3410685676 - Property 1295455071</t>
   </si>
   <si>
-    <t>Gibt an, ob die auf der Finanzierungskostenmitteilung aufgeführte zusätzliche Gebühr im Hauptbuch und den Kundenkonten gebucht werden soll, wenn die Mitteilung ausgestellt wird.</t>
+    <t>Gibt an, ob die in der Verzugszinsmitteilung aufgeführte Zusatzgebühr auf das Hauptbuch und die Kundenkonten gebucht werden soll oder nicht, wenn die Mitteilung ausgestellt wird.</t>
   </si>
   <si>
     <t>Page 3280694829 - Control 650382431 - Property 1295455071</t>
@@ -342,7 +354,7 @@
     <t>Page 3280694829 - Control 2009106446 - Property 1295455071</t>
   </si>
   <si>
-    <t>Gibt an, dass alle Hinweise zu Zeilenkosten der Erinnerung hinzugefügt werden.</t>
+    <t>Gibt an, dass alle Hinweise zu Gebühren im Zusammenhang mit der Leitungsgebühr in die Erinnerung aufgenommen werden.</t>
   </si>
   <si>
     <t>Page 3280694829 - Action 2050659749 - Property 2879900210</t>
@@ -378,7 +390,7 @@
     <t>Table 1909723412 - Field 1840439778 - Property 2879900210</t>
   </si>
   <si>
-    <t>Erinnerungsbedingungen-Code</t>
+    <t>Erinnerungsbedingungscode</t>
   </si>
 </sst>
 </file>
@@ -765,7 +777,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B59"/>
+  <dimension ref="A1:B61"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1071,23 +1083,23 @@
         <v>74</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>15</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>78</v>
+        <v>19</v>
       </c>
     </row>
     <row r="41">
@@ -1127,23 +1139,23 @@
         <v>87</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>91</v>
+        <v>75</v>
       </c>
     </row>
     <row r="48">
@@ -1242,9 +1254,25 @@
         <v>115</v>
       </c>
     </row>
+    <row r="60">
+      <c r="A60" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B59"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B61"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>